<commit_message>
Fixed units on torque rating input
</commit_message>
<xml_diff>
--- a/Torque Curve Predictor.xlsx
+++ b/Torque Curve Predictor.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rcarlyle\Documents\GitHub\StepperSim\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19260" windowHeight="8112"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +24,7 @@
     <author>rcarlyle</author>
   </authors>
   <commentList>
-    <comment ref="D33" authorId="0" shapeId="0">
+    <comment ref="D33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E33" authorId="0" shapeId="0">
+    <comment ref="E33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0">
+    <comment ref="F33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +96,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G33" authorId="0" shapeId="0">
+    <comment ref="G33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -125,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I33" authorId="0" shapeId="0">
+    <comment ref="I33" authorId="0">
       <text>
         <r>
           <rPr>
@@ -154,7 +149,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="68">
   <si>
     <t>Ryan Carlyle</t>
   </si>
@@ -270,9 +265,6 @@
     <t>Low-speed torque</t>
   </si>
   <si>
-    <t>N-cm = Kg-cm * 9.81</t>
-  </si>
-  <si>
     <t>Measured back-emf</t>
   </si>
   <si>
@@ -349,6 +341,18 @@
   </si>
   <si>
     <t>full steps / rev</t>
+  </si>
+  <si>
+    <t>kg-cm</t>
+  </si>
+  <si>
+    <t>oz-in</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Conversion to Nm</t>
   </si>
 </sst>
 </file>
@@ -639,26 +643,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -785,67 +769,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.38113055505954913</c:v>
+                  <c:v>0.38151946378920176</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38109265923325097</c:v>
+                  <c:v>0.38148149893613459</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37550631576183613</c:v>
+                  <c:v>0.37588498001063658</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.35135307605634508</c:v>
+                  <c:v>0.3516877454840534</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.31261329378160935</c:v>
+                  <c:v>0.31287739918514923</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.26816468898049151</c:v>
+                  <c:v>0.26834783181172794</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.22347398874900509</c:v>
+                  <c:v>0.22357572803416911</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.18109116960928826</c:v>
+                  <c:v>0.18111570912464212</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.14198181469351895</c:v>
+                  <c:v>0.14193511701280617</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10634950694324947</c:v>
+                  <c:v>0.10623790546397024</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.405749406070869E-2</c:v>
+                  <c:v>7.3887073087780031E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.4833522844850419E-2</c:v>
+                  <c:v>4.4609870777421831E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.8366596938041345E-2</c:v>
+                  <c:v>1.8094735699324432E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-5.6490109032264696E-3</c:v>
+                  <c:v>-5.964616268332874E-3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2.7495312719101949E-2</c:v>
+                  <c:v>-2.7850710847068912E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-4.7424424279651253E-2</c:v>
+                  <c:v>-4.7816123032640823E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-6.5658112354294959E-2</c:v>
+                  <c:v>-6.6083023539839136E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-8.2389850448530935E-2</c:v>
+                  <c:v>-8.2845238283708433E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-9.7787806356282689E-2</c:v>
+                  <c:v>-9.8271241373685286E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-0.11199800625734471</c:v>
+                  <c:v>-0.11250732497440634</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.12514733226823702</c:v>
+                  <c:v>-0.12568060231656464</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -860,8 +844,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="175981376"/>
-        <c:axId val="175981768"/>
+        <c:axId val="73160192"/>
+        <c:axId val="73166848"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
@@ -979,64 +963,64 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9907929952805992</c:v>
+                  <c:v>3.9948649151272764</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8645858864930238</c:v>
+                  <c:v>7.8725166119744143</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.038082425547895</c:v>
+                  <c:v>11.048596375702591</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.094715028784156</c:v>
+                  <c:v>13.105777850057947</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14.041070280888396</c:v>
+                  <c:v>14.050659617107897</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.041284826445649</c:v>
+                  <c:v>14.047677294262705</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>13.274676055072206</c:v>
+                  <c:v>13.276474895499234</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11.894640692920174</c:v>
+                  <c:v>11.890728557169055</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10.023204891774277</c:v>
+                  <c:v>10.012686700151274</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.7552826428130714</c:v>
+                  <c:v>7.7374362002607278</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.1644510868108489</c:v>
+                  <c:v>5.1386882181044085</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.308014640479819</c:v>
+                  <c:v>2.273851549665864</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-0.76903194999041313</c:v>
+                  <c:v>-0.81199710150332471</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-4.0310233808359515</c:v>
+                  <c:v>-4.0831274677389118</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-7.4494111458838903</c:v>
+                  <c:v>-7.5109390421245061</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-11.001122315777403</c:v>
+                  <c:v>-11.072316868253868</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-14.667336437636434</c:v>
+                  <c:v>-14.748406212029675</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-18.432567243573537</c:v>
+                  <c:v>-18.523692597523141</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-22.283967199402596</c:v>
+                  <c:v>-22.385305088926849</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-26.21079597801695</c:v>
+                  <c:v>-26.322483795763986</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1051,11 +1035,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="175982552"/>
-        <c:axId val="175982160"/>
+        <c:axId val="73175040"/>
+        <c:axId val="73168768"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="175981376"/>
+        <c:axId val="73160192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1200"/>
@@ -1111,26 +1095,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1169,13 +1133,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175981768"/>
+        <c:crossAx val="73166848"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="100"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="175981768"/>
+        <c:axId val="73166848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1236,26 +1200,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
@@ -1294,12 +1238,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175981376"/>
+        <c:crossAx val="73160192"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="175982160"/>
+        <c:axId val="73168768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1341,26 +1285,6 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
@@ -1399,12 +1323,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="175982552"/>
+        <c:crossAx val="73175040"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="175982552"/>
+        <c:axId val="73175040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1414,7 +1338,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175982160"/>
+        <c:crossAx val="73168768"/>
         <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2068,15 +1992,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>297180</xdr:colOff>
+      <xdr:colOff>253637</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>62048</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1562100</xdr:colOff>
+      <xdr:colOff>1518557</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:rowOff>77288</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2353,7 +2277,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2361,9 +2285,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O54"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -2377,12 +2301,12 @@
     <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2391,15 +2315,15 @@
       </c>
       <c r="E2" s="15"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>42760</v>
       </c>
       <c r="N3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -2407,7 +2331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2418,19 +2342,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="O6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="O7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
@@ -2445,7 +2369,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -2458,8 +2382,14 @@
       <c r="F9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2469,8 +2399,15 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P10" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q10">
+        <f>9.81/100</f>
+        <v>9.8100000000000007E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2487,8 +2424,14 @@
       <c r="E11" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2499,42 +2442,51 @@
         <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="P12" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="13">
         <v>200</v>
       </c>
       <c r="C13" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+      <c r="P13" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q13">
+        <v>7.0615518333299997E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" s="13">
-        <v>0.53900000000000003</v>
-      </c>
-      <c r="C14" t="s">
-        <v>20</v>
+        <v>5.5</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>64</v>
       </c>
       <c r="D14">
-        <f>B14/10</f>
-        <v>5.3900000000000003E-2</v>
+        <f>B14*IF(C14=P10,Q10,IF(C14=P11,Q11,IF(C14=P12,Q12,Q13)))</f>
+        <v>0.53955000000000009</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
       </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
@@ -2542,7 +2494,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2561,8 +2513,8 @@
         <v>37</v>
       </c>
       <c r="B17">
-        <f>IF(B16=N4,B14/SQRT(2),B14)</f>
-        <v>0.38113055505954913</v>
+        <f>IF(B16=N4,D14/SQRT(2),D14)</f>
+        <v>0.38151946378920176</v>
       </c>
       <c r="F17" t="s">
         <v>26</v>
@@ -2586,47 +2538,47 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" s="6"/>
       <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" t="s">
+        <v>46</v>
+      </c>
+      <c r="F23" t="s">
         <v>40</v>
-      </c>
-      <c r="D23" t="s">
-        <v>47</v>
-      </c>
-      <c r="F23" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24">
         <f>PI()*SQRT(2)/60*(B17/B12)</f>
-        <v>1.881464933649887E-2</v>
+        <v>1.8833847958270811E-2</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D24">
         <f>IF(B22=O7,B23,B24)</f>
-        <v>1.881464933649887E-2</v>
+        <v>1.8833847958270811E-2</v>
       </c>
       <c r="E24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -2648,7 +2600,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28">
         <f>B27*B10</f>
@@ -2658,29 +2610,29 @@
         <v>16</v>
       </c>
       <c r="F28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="8">
         <f>D30*1000</f>
         <v>1.7142857142857142</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30">
         <f>D11/B10</f>
         <v>1.7142857142857142E-3</v>
       </c>
       <c r="E30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -2688,31 +2640,31 @@
     </row>
     <row r="33" spans="1:9" s="10" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="C33" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="D33" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="F33" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="G33" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="H33" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="10" t="s">
+      <c r="I33" s="10" t="s">
         <v>61</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2731,8 +2683,8 @@
         <v>1</v>
       </c>
       <c r="H34" s="9">
-        <f>$B$17*G34</f>
-        <v>0.38113055505954913</v>
+        <f>$B$17*($B$27/$B$12)*G34</f>
+        <v>0.38151946378920176</v>
       </c>
       <c r="I34" s="9">
         <f>H34*B34</f>
@@ -2749,7 +2701,7 @@
       </c>
       <c r="C35" s="9">
         <f t="shared" ref="C35:C49" si="1">A35*$D$24</f>
-        <v>1.881464933649887</v>
+        <v>1.8833847958270811</v>
       </c>
       <c r="D35" s="9">
         <f>60/(A35*$B$13)</f>
@@ -2757,23 +2709,23 @@
       </c>
       <c r="E35" s="9">
         <f t="shared" ref="E35:E49" si="2">$D$30*$B$28/($B$19-C35)</f>
-        <v>3.2551884554749157E-4</v>
+        <v>3.2554710264351465E-4</v>
       </c>
       <c r="F35" s="9">
         <f t="shared" ref="F35:F49" si="3">D35/E35</f>
-        <v>9.2160562776458832</v>
+        <v>9.215256335072052</v>
       </c>
       <c r="G35" s="12">
         <f>1-EXP(-1*F35)</f>
-        <v>0.99990056996009613</v>
+        <v>0.99990049038995255</v>
       </c>
       <c r="H35" s="9">
-        <f t="shared" ref="H35:H54" si="4">$B$17*G35</f>
-        <v>0.38109265923325097</v>
+        <f t="shared" ref="H35:H54" si="4">$B$17*($B$27/$B$12)*G35</f>
+        <v>0.38148149893613459</v>
       </c>
       <c r="I35" s="9">
         <f t="shared" ref="I35:I54" si="5">H35*B35</f>
-        <v>3.9907929952805992</v>
+        <v>3.9948649151272764</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2786,7 +2738,7 @@
       </c>
       <c r="C36" s="9">
         <f t="shared" si="1"/>
-        <v>3.762929867299774</v>
+        <v>3.7667695916541621</v>
       </c>
       <c r="D36" s="9">
         <f t="shared" ref="D36:D54" si="6">60/(A36*$B$13)</f>
@@ -2794,23 +2746,23 @@
       </c>
       <c r="E36" s="9">
         <f t="shared" si="2"/>
-        <v>3.5578272708388861E-4</v>
+        <v>3.5585024510125326E-4</v>
       </c>
       <c r="F36" s="9">
         <f t="shared" si="3"/>
-        <v>4.2160562776458814</v>
+        <v>4.2152563350720511</v>
       </c>
       <c r="G36" s="12">
         <f t="shared" ref="G36:G54" si="7">1-EXP(-1*F36)</f>
-        <v>0.985243273668168</v>
+        <v>0.9852314644117911</v>
       </c>
       <c r="H36" s="9">
         <f t="shared" si="4"/>
-        <v>0.37550631576183613</v>
+        <v>0.37588498001063658</v>
       </c>
       <c r="I36" s="9">
         <f t="shared" si="5"/>
-        <v>7.8645858864930238</v>
+        <v>7.8725166119744143</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2823,7 +2775,7 @@
       </c>
       <c r="C37" s="9">
         <f t="shared" si="1"/>
-        <v>5.6443948009496605</v>
+        <v>5.6501543874812432</v>
       </c>
       <c r="D37" s="9">
         <f t="shared" si="6"/>
@@ -2831,23 +2783,23 @@
       </c>
       <c r="E37" s="9">
         <f t="shared" si="2"/>
-        <v>3.922507551193411E-4</v>
+        <v>3.9237387343945635E-4</v>
       </c>
       <c r="F37" s="9">
         <f t="shared" si="3"/>
-        <v>2.549389610979214</v>
+        <v>2.5485896684053837</v>
       </c>
       <c r="G37" s="12">
         <f t="shared" si="7"/>
-        <v>0.92187065925860623</v>
+        <v>0.92180813526821515</v>
       </c>
       <c r="H37" s="9">
         <f t="shared" si="4"/>
-        <v>0.35135307605634508</v>
+        <v>0.3516877454840534</v>
       </c>
       <c r="I37" s="9">
         <f t="shared" si="5"/>
-        <v>11.038082425547895</v>
+        <v>11.048596375702591</v>
       </c>
     </row>
     <row r="38" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2860,7 +2812,7 @@
       </c>
       <c r="C38" s="9">
         <f t="shared" si="1"/>
-        <v>7.5258597345995479</v>
+        <v>7.5335391833083243</v>
       </c>
       <c r="D38" s="9">
         <f t="shared" si="6"/>
@@ -2868,23 +2820,23 @@
       </c>
       <c r="E38" s="9">
         <f t="shared" si="2"/>
-        <v>4.3704860369082101E-4</v>
+        <v>4.3725242966002279E-4</v>
       </c>
       <c r="F38" s="9">
         <f t="shared" si="3"/>
-        <v>1.7160562776458808</v>
+        <v>1.71525633507205</v>
       </c>
       <c r="G38" s="12">
         <f t="shared" si="7"/>
-        <v>0.82022627058270248</v>
+        <v>0.82008240438821001</v>
       </c>
       <c r="H38" s="9">
         <f t="shared" si="4"/>
-        <v>0.31261329378160935</v>
+        <v>0.31287739918514923</v>
       </c>
       <c r="I38" s="9">
         <f t="shared" si="5"/>
-        <v>13.094715028784156</v>
+        <v>13.105777850057947</v>
       </c>
     </row>
     <row r="39" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2897,7 +2849,7 @@
       </c>
       <c r="C39" s="9">
         <f t="shared" si="1"/>
-        <v>9.4073246682494354</v>
+        <v>9.4169239791354045</v>
       </c>
       <c r="D39" s="9">
         <f t="shared" si="6"/>
@@ -2905,23 +2857,23 @@
       </c>
       <c r="E39" s="9">
         <f t="shared" si="2"/>
-        <v>4.9339821768900228E-4</v>
+        <v>4.9372299710285182E-4</v>
       </c>
       <c r="F39" s="9">
         <f t="shared" si="3"/>
-        <v>1.2160562776458805</v>
+        <v>1.2152563350720498</v>
       </c>
       <c r="G39" s="12">
         <f t="shared" si="7"/>
-        <v>0.70360322839661216</v>
+        <v>0.70336603314161783</v>
       </c>
       <c r="H39" s="9">
         <f t="shared" si="4"/>
-        <v>0.26816468898049151</v>
+        <v>0.26834783181172794</v>
       </c>
       <c r="I39" s="9">
         <f t="shared" si="5"/>
-        <v>14.041070280888396</v>
+        <v>14.050659617107897</v>
       </c>
     </row>
     <row r="40" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2934,7 +2886,7 @@
       </c>
       <c r="C40" s="9">
         <f t="shared" si="1"/>
-        <v>11.288789601899321</v>
+        <v>11.300308774962486</v>
       </c>
       <c r="D40" s="9">
         <f t="shared" si="6"/>
@@ -2942,23 +2894,23 @@
       </c>
       <c r="E40" s="9">
         <f t="shared" si="2"/>
-        <v>5.6642914203322678E-4</v>
+        <v>5.6694291793529252E-4</v>
       </c>
       <c r="F40" s="9">
         <f t="shared" si="3"/>
-        <v>0.88272294431254739</v>
+        <v>0.88192300173871652</v>
       </c>
       <c r="G40" s="12">
         <f t="shared" si="7"/>
-        <v>0.5863449827949081</v>
+        <v>0.58601395014986657</v>
       </c>
       <c r="H40" s="9">
         <f t="shared" si="4"/>
-        <v>0.22347398874900509</v>
+        <v>0.22357572803416911</v>
       </c>
       <c r="I40" s="9">
         <f t="shared" si="5"/>
-        <v>14.041284826445649</v>
+        <v>14.047677294262705</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -2971,7 +2923,7 @@
       </c>
       <c r="C41" s="9">
         <f t="shared" si="1"/>
-        <v>13.170254535549208</v>
+        <v>13.183693570789568</v>
       </c>
       <c r="D41" s="9">
         <f t="shared" si="6"/>
@@ -2979,23 +2931,23 @@
       </c>
       <c r="E41" s="9">
         <f t="shared" si="2"/>
-        <v>6.6483557010960006E-4</v>
+        <v>6.6566161444499533E-4</v>
       </c>
       <c r="F41" s="9">
         <f t="shared" si="3"/>
-        <v>0.64462770621730925</v>
+        <v>0.64382776364347816</v>
       </c>
       <c r="G41" s="12">
         <f t="shared" si="7"/>
-        <v>0.47514209292664544</v>
+        <v>0.47472206876635969</v>
       </c>
       <c r="H41" s="9">
         <f t="shared" si="4"/>
-        <v>0.18109116960928826</v>
+        <v>0.18111570912464212</v>
       </c>
       <c r="I41" s="9">
         <f t="shared" si="5"/>
-        <v>13.274676055072206</v>
+        <v>13.276474895499234</v>
       </c>
     </row>
     <row r="42" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3008,7 +2960,7 @@
       </c>
       <c r="C42" s="9">
         <f t="shared" si="1"/>
-        <v>15.051719469199096</v>
+        <v>15.067078366616649</v>
       </c>
       <c r="D42" s="9">
         <f t="shared" si="6"/>
@@ -3016,23 +2968,23 @@
       </c>
       <c r="E42" s="9">
         <f t="shared" si="2"/>
-        <v>8.046238576469363E-4</v>
+        <v>8.0600729475704491E-4</v>
       </c>
       <c r="F42" s="9">
         <f t="shared" si="3"/>
-        <v>0.46605627764588053</v>
+        <v>0.46525633507204966</v>
       </c>
       <c r="G42" s="12">
         <f t="shared" si="7"/>
-        <v>0.37252802959168474</v>
+        <v>0.37202588723292129</v>
       </c>
       <c r="H42" s="9">
         <f t="shared" si="4"/>
-        <v>0.14198181469351895</v>
+        <v>0.14193511701280617</v>
       </c>
       <c r="I42" s="9">
         <f t="shared" si="5"/>
-        <v>11.894640692920174</v>
+        <v>11.890728557169055</v>
       </c>
     </row>
     <row r="43" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3045,7 +2997,7 @@
       </c>
       <c r="C43" s="9">
         <f t="shared" si="1"/>
-        <v>16.933184402848983</v>
+        <v>16.950463162443729</v>
       </c>
       <c r="D43" s="9">
         <f t="shared" si="6"/>
@@ -3053,23 +3005,23 @@
       </c>
       <c r="E43" s="9">
         <f t="shared" si="2"/>
-        <v>1.0188464522694883E-3</v>
+        <v>1.0213436947576666E-3</v>
       </c>
       <c r="F43" s="9">
         <f t="shared" si="3"/>
-        <v>0.32716738875699158</v>
+        <v>0.32636744618316077</v>
       </c>
       <c r="G43" s="12">
         <f t="shared" si="7"/>
-        <v>0.27903694818336744</v>
+        <v>0.27845998840748298</v>
       </c>
       <c r="H43" s="9">
         <f t="shared" si="4"/>
-        <v>0.10634950694324947</v>
+        <v>0.10623790546397024</v>
       </c>
       <c r="I43" s="9">
         <f t="shared" si="5"/>
-        <v>10.023204891774277</v>
+        <v>10.012686700151274</v>
       </c>
     </row>
     <row r="44" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3082,7 +3034,7 @@
       </c>
       <c r="C44" s="9">
         <f t="shared" si="1"/>
-        <v>18.814649336498871</v>
+        <v>18.833847958270809</v>
       </c>
       <c r="D44" s="9">
         <f t="shared" si="6"/>
@@ -3090,23 +3042,23 @@
       </c>
       <c r="E44" s="9">
         <f t="shared" si="2"/>
-        <v>1.3885271155680309E-3</v>
+        <v>1.3936872050691808E-3</v>
       </c>
       <c r="F44" s="9">
         <f t="shared" si="3"/>
-        <v>0.21605627764588042</v>
+        <v>0.21525633507204966</v>
       </c>
       <c r="G44" s="12">
         <f t="shared" si="7"/>
-        <v>0.19431004173658473</v>
+        <v>0.1936652781851369</v>
       </c>
       <c r="H44" s="9">
         <f t="shared" si="4"/>
-        <v>7.405749406070869E-2</v>
+        <v>7.3887073087780031E-2</v>
       </c>
       <c r="I44" s="9">
         <f t="shared" si="5"/>
-        <v>7.7552826428130714</v>
+        <v>7.7374362002607278</v>
       </c>
     </row>
     <row r="45" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3119,7 +3071,7 @@
       </c>
       <c r="C45" s="9">
         <f t="shared" si="1"/>
-        <v>20.696114270148758</v>
+        <v>20.717232754097893</v>
       </c>
       <c r="D45" s="9">
         <f t="shared" si="6"/>
@@ -3127,23 +3079,23 @@
       </c>
       <c r="E45" s="9">
         <f t="shared" si="2"/>
-        <v>2.179252125745941E-3</v>
+        <v>2.1932715482609342E-3</v>
       </c>
       <c r="F45" s="9">
         <f t="shared" si="3"/>
-        <v>0.12514718673678948</v>
+        <v>0.12434724416295866</v>
       </c>
       <c r="G45" s="12">
         <f t="shared" si="7"/>
-        <v>0.11763297969601383</v>
+        <v>0.11692685435852312</v>
       </c>
       <c r="H45" s="9">
         <f t="shared" si="4"/>
-        <v>4.4833522844850419E-2</v>
+        <v>4.4609870777421831E-2</v>
       </c>
       <c r="I45" s="9">
         <f t="shared" si="5"/>
-        <v>5.1644510868108489</v>
+        <v>5.1386882181044085</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3156,7 +3108,7 @@
       </c>
       <c r="C46" s="9">
         <f t="shared" si="1"/>
-        <v>22.577579203798642</v>
+        <v>22.600617549924973</v>
       </c>
       <c r="D46" s="9">
         <f t="shared" si="6"/>
@@ -3164,23 +3116,23 @@
       </c>
       <c r="E46" s="9">
         <f t="shared" si="2"/>
-        <v>5.0617932606356279E-3</v>
+        <v>5.1451266947173547E-3</v>
       </c>
       <c r="F46" s="9">
         <f t="shared" si="3"/>
-        <v>4.9389610979213835E-2</v>
+        <v>4.8589668405382903E-2</v>
       </c>
       <c r="G46" s="12">
         <f t="shared" si="7"/>
-        <v>4.8189778264226768E-2</v>
+        <v>4.742808012888744E-2</v>
       </c>
       <c r="H46" s="9">
         <f t="shared" si="4"/>
-        <v>1.8366596938041345E-2</v>
+        <v>1.8094735699324432E-2</v>
       </c>
       <c r="I46" s="9">
         <f t="shared" si="5"/>
-        <v>2.308014640479819</v>
+        <v>2.273851549665864</v>
       </c>
     </row>
     <row r="47" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3193,7 +3145,7 @@
       </c>
       <c r="C47" s="9">
         <f t="shared" si="1"/>
-        <v>24.459044137448529</v>
+        <v>24.484002345752053</v>
       </c>
       <c r="D47" s="9">
         <f t="shared" si="6"/>
@@ -3201,23 +3153,23 @@
       </c>
       <c r="E47" s="9">
         <f t="shared" si="2"/>
-        <v>-1.5684766262388662E-2</v>
+        <v>-1.4875960960090981E-2</v>
       </c>
       <c r="F47" s="9">
         <f t="shared" si="3"/>
-        <v>-1.4712953123350305E-2</v>
+        <v>-1.5512895697181192E-2</v>
       </c>
       <c r="G47" s="12">
         <f t="shared" si="7"/>
-        <v>-1.4821721397655585E-2</v>
+        <v>-1.5633845280377257E-2</v>
       </c>
       <c r="H47" s="9">
         <f t="shared" si="4"/>
-        <v>-5.6490109032264696E-3</v>
+        <v>-5.964616268332874E-3</v>
       </c>
       <c r="I47" s="9">
         <f t="shared" si="5"/>
-        <v>-0.76903194999041313</v>
+        <v>-0.81199710150332471</v>
       </c>
     </row>
     <row r="48" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3230,7 +3182,7 @@
       </c>
       <c r="C48" s="9">
         <f t="shared" si="1"/>
-        <v>26.340509071098417</v>
+        <v>26.367387141579137</v>
       </c>
       <c r="D48" s="9">
         <f t="shared" si="6"/>
@@ -3238,23 +3190,23 @@
       </c>
       <c r="E48" s="9">
         <f t="shared" si="2"/>
-        <v>-3.0762538325138766E-3</v>
+        <v>-3.0413276618531117E-3</v>
       </c>
       <c r="F48" s="9">
         <f t="shared" si="3"/>
-        <v>-6.9658008068405275E-2</v>
+        <v>-7.0457950642236228E-2</v>
       </c>
       <c r="G48" s="12">
         <f t="shared" si="7"/>
-        <v>-7.2141454821972983E-2</v>
+        <v>-7.2999449544354222E-2</v>
       </c>
       <c r="H48" s="9">
         <f t="shared" si="4"/>
-        <v>-2.7495312719101949E-2</v>
+        <v>-2.7850710847068912E-2</v>
       </c>
       <c r="I48" s="9">
         <f t="shared" si="5"/>
-        <v>-4.0310233808359515</v>
+        <v>-4.0831274677389118</v>
       </c>
     </row>
     <row r="49" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
@@ -3267,7 +3219,7 @@
       </c>
       <c r="C49" s="9">
         <f t="shared" si="1"/>
-        <v>28.221974004748304</v>
+        <v>28.250771937406217</v>
       </c>
       <c r="D49" s="9">
         <f t="shared" si="6"/>
@@ -3275,23 +3227,23 @@
       </c>
       <c r="E49" s="9">
         <f t="shared" si="2"/>
-        <v>-1.7053634133944013E-3</v>
+        <v>-1.693809996401118E-3</v>
       </c>
       <c r="F49" s="9">
         <f t="shared" si="3"/>
-        <v>-0.11727705568745293</v>
+        <v>-0.11807699826128384</v>
       </c>
       <c r="G49" s="12">
         <f t="shared" si="7"/>
-        <v>-0.12443091651951521</v>
+        <v>-0.12533075654315851</v>
       </c>
       <c r="H49" s="9">
         <f t="shared" si="4"/>
-        <v>-4.7424424279651253E-2</v>
+        <v>-4.7816123032640823E-2</v>
       </c>
       <c r="I49" s="9">
         <f t="shared" si="5"/>
-        <v>-7.4494111458838903</v>
+        <v>-7.5109390421245061</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
@@ -3304,7 +3256,7 @@
       </c>
       <c r="C50" s="9">
         <f t="shared" ref="C50:C54" si="8">A50*$D$24</f>
-        <v>30.103438938398192</v>
+        <v>30.134156733233297</v>
       </c>
       <c r="D50" s="9">
         <f t="shared" si="6"/>
@@ -3312,23 +3264,23 @@
       </c>
       <c r="E50" s="9">
         <f t="shared" ref="E50:E53" si="9">$D$30*$B$28/($B$19-C50)</f>
-        <v>-1.1796628216763304E-3</v>
+        <v>-1.1737554668259833E-3</v>
       </c>
       <c r="F50" s="9">
         <f t="shared" ref="F50:F53" si="10">D50/E50</f>
-        <v>-0.15894372235411963</v>
+        <v>-0.1597436649279505</v>
       </c>
       <c r="G50" s="12">
         <f t="shared" si="7"/>
-        <v>-0.17227197211736622</v>
+        <v>-0.17321009754918171</v>
       </c>
       <c r="H50" s="9">
         <f t="shared" si="4"/>
-        <v>-6.5658112354294959E-2</v>
+        <v>-6.6083023539839136E-2</v>
       </c>
       <c r="I50" s="9">
         <f t="shared" si="5"/>
-        <v>-11.001122315777403</v>
+        <v>-11.072316868253868</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
@@ -3341,7 +3293,7 @@
       </c>
       <c r="C51" s="9">
         <f t="shared" si="8"/>
-        <v>31.984903872048079</v>
+        <v>32.017541529060381</v>
       </c>
       <c r="D51" s="9">
         <f t="shared" si="6"/>
@@ -3349,23 +3301,23 @@
       </c>
       <c r="E51" s="9">
         <f t="shared" si="9"/>
-        <v>-9.0170152519985711E-4</v>
+        <v>-8.9803089561842347E-4</v>
       </c>
       <c r="F51" s="9">
         <f t="shared" si="10"/>
-        <v>-0.19570842823647261</v>
+        <v>-0.19650837081030351</v>
       </c>
       <c r="G51" s="12">
         <f t="shared" si="7"/>
-        <v>-0.21617225214508995</v>
+        <v>-0.21714550932972143</v>
       </c>
       <c r="H51" s="9">
         <f t="shared" si="4"/>
-        <v>-8.2389850448530935E-2</v>
+        <v>-8.2845238283708433E-2</v>
       </c>
       <c r="I51" s="9">
         <f t="shared" si="5"/>
-        <v>-14.667336437636434</v>
+        <v>-14.748406212029675</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
@@ -3378,7 +3330,7 @@
       </c>
       <c r="C52" s="9">
         <f t="shared" si="8"/>
-        <v>33.866368805697967</v>
+        <v>33.900926324887457</v>
       </c>
       <c r="D52" s="9">
         <f t="shared" si="6"/>
@@ -3386,23 +3338,23 @@
       </c>
       <c r="E52" s="9">
         <f t="shared" si="9"/>
-        <v>-7.2975175992224183E-4</v>
+        <v>-7.2720468406089664E-4</v>
       </c>
       <c r="F52" s="9">
         <f t="shared" si="10"/>
-        <v>-0.22838816679856408</v>
+        <v>-0.22918810937239489</v>
       </c>
       <c r="G52" s="12">
         <f t="shared" si="7"/>
-        <v>-0.25657299069344885</v>
+        <v>-0.25757857907868731</v>
       </c>
       <c r="H52" s="9">
         <f t="shared" si="4"/>
-        <v>-9.7787806356282689E-2</v>
+        <v>-9.8271241373685286E-2</v>
       </c>
       <c r="I52" s="9">
         <f t="shared" si="5"/>
-        <v>-18.432567243573537</v>
+        <v>-18.523692597523141</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
@@ -3415,7 +3367,7 @@
       </c>
       <c r="C53" s="9">
         <f t="shared" si="8"/>
-        <v>35.747833739347854</v>
+        <v>35.784311120714541</v>
       </c>
       <c r="D53" s="9">
         <f t="shared" si="6"/>
@@ -3423,23 +3375,23 @@
       </c>
       <c r="E53" s="9">
         <f t="shared" si="9"/>
-        <v>-6.1287894940873454E-4</v>
+        <v>-6.1098183222129884E-4</v>
       </c>
       <c r="F53" s="9">
         <f t="shared" si="10"/>
-        <v>-0.25762793288043545</v>
+        <v>-0.25842787545426632</v>
       </c>
       <c r="G53" s="12">
         <f t="shared" si="7"/>
-        <v>-0.2938573272873537</v>
+        <v>-0.29489275293322703</v>
       </c>
       <c r="H53" s="9">
         <f t="shared" si="4"/>
-        <v>-0.11199800625734471</v>
+        <v>-0.11250732497440634</v>
       </c>
       <c r="I53" s="9">
         <f t="shared" si="5"/>
-        <v>-22.283967199402596</v>
+        <v>-22.385305088926849</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -3452,7 +3404,7 @@
       </c>
       <c r="C54" s="9">
         <f t="shared" si="8"/>
-        <v>37.629298672997741</v>
+        <v>37.667695916541618</v>
       </c>
       <c r="D54" s="9">
         <f t="shared" si="6"/>
@@ -3460,27 +3412,27 @@
       </c>
       <c r="E54" s="9">
         <f>$D$30*$B$28/($B$19-C54)</f>
-        <v>-5.2827369718330274E-4</v>
+        <v>-5.2678959525914281E-4</v>
       </c>
       <c r="F54" s="9">
         <f>D54/E54</f>
-        <v>-0.28394372235411963</v>
+        <v>-0.28474366492795045</v>
       </c>
       <c r="G54" s="12">
         <f t="shared" si="7"/>
-        <v>-0.32835817177839122</v>
+        <v>-0.3294212071602356</v>
       </c>
       <c r="H54" s="9">
         <f t="shared" si="4"/>
-        <v>-0.12514733226823702</v>
+        <v>-0.12568060231656464</v>
       </c>
       <c r="I54" s="9">
         <f t="shared" si="5"/>
-        <v>-26.21079597801695</v>
+        <v>-26.322483795763986</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="B5XFPmJa0BZphMKG/9BOSJA8KbdYOfZtO5/cJGR9LQ18dSOAeQZisbvw/CzCy4wpKcQ3ip0ou9kphxLhA/2kaQ==" saltValue="EzNdNvzTC06a273MuV86wg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection password="D05D" sheet="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="D2:E2"/>
   </mergeCells>
@@ -3499,12 +3451,15 @@
       <formula>$B$19</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16">
       <formula1>$N$4:$N$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B22">
       <formula1>$O$6:$O$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14">
+      <formula1>$P$10:$P$13</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>